<commit_message>
Made starter decks for three of the mythologys.
</commit_message>
<xml_diff>
--- a/Spells.xlsx
+++ b/Spells.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{E150C852-A2A5-4905-A61C-CB040E18100D}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{E150C852-A2A5-4905-A61C-CB040E18100D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t>WATER</t>
   </si>
@@ -156,6 +156,117 @@
   </si>
   <si>
     <t>medusa's head was an idea for a card</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>Adrenaline Rush</t>
+  </si>
+  <si>
+    <t>Cure</t>
+  </si>
+  <si>
+    <t>Circle of Protection</t>
+  </si>
+  <si>
+    <t>Guardian Circle</t>
+  </si>
+  <si>
+    <t>God's name + Aura</t>
+  </si>
+  <si>
+    <t>Familiar</t>
+  </si>
+  <si>
+    <t>Ash Shell</t>
+  </si>
+  <si>
+    <t>Cloud's Call</t>
+  </si>
+  <si>
+    <t>Rising Tide</t>
+  </si>
+  <si>
+    <t>Styx burn</t>
+  </si>
+  <si>
+    <t>Mesmerize</t>
+  </si>
+  <si>
+    <t>You've got mail</t>
+  </si>
+  <si>
+    <t>War Chant/Song</t>
+  </si>
+  <si>
+    <t>Stone Heart</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>Freeze</t>
+  </si>
+  <si>
+    <t>Pacify</t>
+  </si>
+  <si>
+    <t>Seduction</t>
+  </si>
+  <si>
+    <t>Aristocracy</t>
+  </si>
+  <si>
+    <t>Overlord</t>
+  </si>
+  <si>
+    <t>Conquering Hero</t>
+  </si>
+  <si>
+    <t>Vanquisher</t>
+  </si>
+  <si>
+    <t>Authority</t>
+  </si>
+  <si>
+    <t>Awe</t>
+  </si>
+  <si>
+    <t>Coronation</t>
+  </si>
+  <si>
+    <t>pull rank</t>
+  </si>
+  <si>
+    <t>Allegiance</t>
+  </si>
+  <si>
+    <t>calm</t>
+  </si>
+  <si>
+    <t>rain</t>
+  </si>
+  <si>
+    <t>typhoon</t>
+  </si>
+  <si>
+    <t>WaterWell</t>
+  </si>
+  <si>
+    <t>Soak</t>
+  </si>
+  <si>
+    <t>steam</t>
+  </si>
+  <si>
+    <t>after life</t>
+  </si>
+  <si>
+    <t>Blood Shed</t>
+  </si>
+  <si>
+    <t>Eternal rest</t>
   </si>
 </sst>
 </file>
@@ -507,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E83FCF-0584-4882-A42B-1EE4AEDD83F0}">
-  <dimension ref="A2:G20"/>
+  <dimension ref="A2:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -521,7 +632,7 @@
     <col min="4" max="4" width="16.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -535,7 +646,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -549,7 +660,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -569,7 +680,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -589,7 +700,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -606,7 +717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -614,84 +725,213 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" t="s">
+        <v>75</v>
+      </c>
+      <c r="O11" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N13" t="s">
+        <v>61</v>
+      </c>
+      <c r="O13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" t="s">
+        <v>66</v>
+      </c>
+      <c r="N14" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="I17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="I18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -699,7 +939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>35</v>
       </c>

</xml_diff>